<commit_message>
till chapter 9 practiced exercise cleaned data and report are added to codebase
</commit_message>
<xml_diff>
--- a/excel_mother_of_business/chapter-5/Loan_repayment.xlsx
+++ b/excel_mother_of_business/chapter-5/Loan_repayment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\academic\projects\data-analysis\practice-work\excel_mother_of_business\chapter-5\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\data-analysis-practice\excel_mother_of_business\chapter-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01D24FF-9E05-4513-9752-4B3E100C3808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E6007-521E-431C-AEDC-4718624EFDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65720D13-8C9D-471F-8249-A5903CDD542C}"/>
   </bookViews>
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -197,32 +197,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -259,16 +264,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{E1BF8FF4-C320-4640-9C6E-EBA32844847E}"/>
@@ -289,16 +284,99 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1005840</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAFF717E-04FB-C798-E9B3-F863F3E44D02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="525780"/>
+          <a:ext cx="3558540" cy="2644140"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1600" u="sng"/>
+            <a:t>MY FINDINGS</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-IN" sz="1600"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-IN" sz="1600"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1600"/>
+            <a:t>As Mr. Hathodwala's</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1600" baseline="0"/>
+            <a:t> monthly budget is 25000 for loan emi repayment, I will suggest him to go for Y Axis Bank as it's EMI is under the budget and if we consider the interest also we can find the lowest interest amount he will pay.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B0E9431-9F7B-4E71-9E12-02DA71CD026C}" name="Table1" displayName="Table1" ref="A3:D6" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B0E9431-9F7B-4E71-9E12-02DA71CD026C}" name="Table1" displayName="Table1" ref="A3:D6" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A3:D6" xr:uid="{2B0E9431-9F7B-4E71-9E12-02DA71CD026C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{04005065-FB0F-4A74-9128-801E600952E0}" name="Bank"/>
-    <tableColumn id="2" xr3:uid="{DC5EBE56-09B0-42CD-ABB0-3A7830F50E47}" name="Left Join Bank" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B4772C65-39FD-459F-92A3-3D16A1243589}" name="Y Axis Bank" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{C69C4136-3C97-41A9-A6CE-97F8A35117C6}" name="CBI Bank" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{DC5EBE56-09B0-42CD-ABB0-3A7830F50E47}" name="Left Join Bank" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B4772C65-39FD-459F-92A3-3D16A1243589}" name="Y Axis Bank" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C69C4136-3C97-41A9-A6CE-97F8A35117C6}" name="CBI Bank" dataDxfId="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -602,7 +680,7 @@
   <dimension ref="A2:F138"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,38 +694,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="2">
         <v>1500000</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="2">
         <v>1500000</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="2">
         <v>1500000</v>
       </c>
     </row>
@@ -655,13 +733,13 @@
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>0.15</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>0.125</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>0.11</v>
       </c>
     </row>
@@ -669,13 +747,13 @@
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6">
         <v>8</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6">
         <v>10</v>
       </c>
     </row>
@@ -686,62 +764,62 @@
       <c r="D7" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="10">
         <f>ABS(PMT(B5/12,B6*12,B4))</f>
         <v>35684.895129538098</v>
       </c>
-      <c r="C10" s="14">
-        <f t="shared" ref="C10:D10" si="0">ABS(PMT(C5/12,C6*12,C4))</f>
+      <c r="C10" s="10">
+        <f>ABS(PMT(C5/12,C6*12,C4))</f>
         <v>24793.212974723752</v>
       </c>
-      <c r="D10" s="12">
-        <f t="shared" si="0"/>
+      <c r="D10" s="11">
+        <f t="shared" ref="C10:D10" si="0">ABS(PMT(D5/12,D6*12,D4))</f>
         <v>20662.501693788374</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="13">
         <f>B10*B6*12</f>
         <v>2141093.7077722857</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <f t="shared" ref="C11:D11" si="1">C10*C6*12</f>
         <v>2380148.4455734803</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <f t="shared" si="1"/>
         <v>2479500.2032546047</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="10">
         <f>B11-B4</f>
         <v>641093.70777228568</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="10">
         <f t="shared" ref="C12:D12" si="2">C11-C4</f>
         <v>880148.44557348033</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <f t="shared" si="2"/>
         <v>979500.20325460471</v>
       </c>
@@ -1584,7 +1662,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F1:F9 F11:F16 F21:F1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1594,34 +1672,15 @@
     <oddHeader xml:space="preserve">&amp;L&amp;"-,Bold"&amp;20Loan Repayment Report&amp;R&amp;G
 </oddHeader>
   </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawingHF r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100686C0266E115364AA9B96DE5BECF7DB6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c921848065db5a49d1de2391ec81580e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="631564f6-0349-4cc5-b00d-7cf3ba42f824" xmlns:ns3="46297aa2-77d1-4586-9726-07d56a535ee7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff9dd1b7eff9d7fccc1b7fb333026bb0" ns2:_="" ns3:_="">
     <xsd:import namespace="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
@@ -1850,26 +1909,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6029F160-14CD-4DAE-A1B5-794886BB718A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
-    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB7CC7E-D5A6-4098-8B4D-E260951D10E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBD461B2-3FEB-416A-9AEA-0E5BA44BF08F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1886,4 +1946,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB7CC7E-D5A6-4098-8B4D-E260951D10E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6029F160-14CD-4DAE-A1B5-794886BB718A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
+    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>